<commit_message>
24.04.2020(super_admin course list page done)
</commit_message>
<xml_diff>
--- a/excel_files/demo/insert_multiple_course.xlsx
+++ b/excel_files/demo/insert_multiple_course.xlsx
@@ -272,14 +272,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -618,12 +618,12 @@
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -1998,9 +1998,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="10"/>
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="9"/>
       <c r="D101" s="7" t="s">
         <v>0</v>
       </c>

</xml_diff>